<commit_message>
Update comparison excel sheet to include PPL update results
</commit_message>
<xml_diff>
--- a/src/games/results/PROFILE LIKELIHOOD RESULTS.xlsx
+++ b/src/games/results/PROFILE LIKELIHOOD RESULTS.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kdreyer/Documents/Github/GAMES/src/games/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{71342F67-B409-024A-9A22-381A99081DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801DE8A1-6951-604A-B972-B61C963B95F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2780" yWindow="-21100" windowWidth="28040" windowHeight="20440" xr2:uid="{F44A9B0A-B80B-5A4A-9ADC-C0D98F2F313F}"/>
+    <workbookView xWindow="32400" yWindow="500" windowWidth="34800" windowHeight="21100" xr2:uid="{F44A9B0A-B80B-5A4A-9ADC-C0D98F2F313F}"/>
   </bookViews>
   <sheets>
     <sheet name="PROFILE LIKELIHOOD RESULTS m" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="69">
   <si>
     <t>Kate's original PPL</t>
   </si>
@@ -182,6 +195,51 @@
   </si>
   <si>
     <t>[1, 1559.86711, 0.04209]</t>
+  </si>
+  <si>
+    <t>PPL update</t>
+  </si>
+  <si>
+    <t>[1, 1052.78824, 0.02988]</t>
+  </si>
+  <si>
+    <t>[1, 4535.08779, 0.02887]</t>
+  </si>
+  <si>
+    <t>[1, 1732.7299, 0.01887]</t>
+  </si>
+  <si>
+    <t>[1, 1686.72057, 0.02177]</t>
+  </si>
+  <si>
+    <t>[1, 1655.92706, 0.02468]</t>
+  </si>
+  <si>
+    <t>[1, 1593.77553, 0.03338]</t>
+  </si>
+  <si>
+    <t>[1, 1580.3565, 0.03629]</t>
+  </si>
+  <si>
+    <t>[1, 1569.21502, 0.03919]</t>
+  </si>
+  <si>
+    <t>[1, 1559.87949, 0.04209]</t>
+  </si>
+  <si>
+    <t>fixed m difference (update -my original)</t>
+  </si>
+  <si>
+    <t>fixed m ppl difference (update - my original)</t>
+  </si>
+  <si>
+    <t>fixed w difference (update -my original)</t>
+  </si>
+  <si>
+    <t>fixed w ppl difference (update - my original)</t>
+  </si>
+  <si>
+    <t>fixed m difference (my original - Kate's original)</t>
   </si>
 </sst>
 </file>
@@ -686,14 +744,14 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1069,10 +1127,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A6246EA-01B8-AE45-8EE2-E95FFB54209D}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1081,39 +1139,41 @@
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="H2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
@@ -1411,23 +1471,23 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>3</v>
       </c>
@@ -1437,18 +1497,30 @@
       <c r="D19" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4" t="s">
+      <c r="H19" s="2"/>
+      <c r="I19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N19" t="s">
+        <v>68</v>
+      </c>
+      <c r="O19" t="s">
+        <v>65</v>
+      </c>
+      <c r="P19" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>0</v>
       </c>
@@ -1461,20 +1533,36 @@
       <c r="D20" t="s">
         <v>33</v>
       </c>
-      <c r="H20" s="4">
-        <v>0</v>
-      </c>
-      <c r="I20" s="4">
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2">
         <v>1.8869500000000001E-2</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="2">
         <v>18.783000000000001</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N20">
+        <f>B20-B4</f>
+        <v>-2.2000000058142177E-5</v>
+      </c>
+      <c r="O20">
+        <f>C20-C4</f>
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <f>I20-I4</f>
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <f>J20-J4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1487,20 +1575,36 @@
       <c r="D21" t="s">
         <v>35</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="2">
         <v>1</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="2">
         <v>2.17725E-2</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="2">
         <v>12.215999999999999</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N21">
+        <f t="shared" ref="N21:N31" si="0">B21-B5</f>
+        <v>-2.6500009880692232E-5</v>
+      </c>
+      <c r="O21">
+        <f t="shared" ref="O21:O31" si="1">C21-C5</f>
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <f t="shared" ref="P21:P31" si="2">I21-I5</f>
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" ref="Q21:Q31" si="3">J21-J5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1513,20 +1617,36 @@
       <c r="D22" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="2">
         <v>2</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="2">
         <v>2.46755E-2</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="2">
         <v>8.1630000000000003</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="K22" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>-3.0500009870593203E-5</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1539,20 +1659,36 @@
       <c r="D23" t="s">
         <v>38</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="2">
         <v>3</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="2">
         <v>2.903E-2</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="2">
         <v>6.0439999999999996</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="K23" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N23">
+        <f t="shared" si="0"/>
+        <v>-3.450000008342613E-5</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>4</v>
       </c>
@@ -1565,20 +1701,36 @@
       <c r="D24" t="s">
         <v>39</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24" s="2">
         <v>4</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I24" s="2">
         <v>2.903E-2</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J24" s="2">
         <v>6.0439999999999996</v>
       </c>
-      <c r="K24" s="4" t="s">
+      <c r="K24" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N24">
+        <f t="shared" si="0"/>
+        <v>-4.0000000126383384E-5</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>5</v>
       </c>
@@ -1591,20 +1743,36 @@
       <c r="D25" t="s">
         <v>39</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25" s="2">
         <v>5</v>
       </c>
-      <c r="I25" s="4">
+      <c r="I25" s="2">
         <v>3.3384499999999998E-2</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J25" s="2">
         <v>7.9050000000000002</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="K25" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N25">
+        <f t="shared" si="0"/>
+        <v>-4.0000000126383384E-5</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>6</v>
       </c>
@@ -1617,20 +1785,36 @@
       <c r="D26" t="s">
         <v>40</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26" s="2">
         <v>6</v>
       </c>
-      <c r="I26" s="4">
+      <c r="I26" s="2">
         <v>3.62875E-2</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J26" s="2">
         <v>11.025</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="K26" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N26">
+        <f t="shared" si="0"/>
+        <v>-5.1999999868712621E-5</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1643,20 +1827,36 @@
       <c r="D27" t="s">
         <v>41</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="2">
         <v>7</v>
       </c>
-      <c r="I27" s="4">
+      <c r="I27" s="2">
         <v>3.9190500000000003E-2</v>
       </c>
-      <c r="J27" s="4">
+      <c r="J27" s="2">
         <v>15.467000000000001</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="K27" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N27">
+        <f t="shared" si="0"/>
+        <v>-6.3999999838415533E-5</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>8</v>
       </c>
@@ -1669,20 +1869,36 @@
       <c r="D28" t="s">
         <v>42</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28" s="2">
         <v>8</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="I28" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J28" s="2">
         <v>21.103000000000002</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="K28" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N28">
+        <f t="shared" si="0"/>
+        <v>-7.5999999808118446E-5</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>9</v>
       </c>
@@ -1695,8 +1911,24 @@
       <c r="D29" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N29">
+        <f t="shared" si="0"/>
+        <v>-8.799999022812699E-5</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>10</v>
       </c>
@@ -1709,8 +1941,24 @@
       <c r="D30" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N30">
+        <f t="shared" si="0"/>
+        <v>-9.9999990197829902E-5</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>11</v>
       </c>
@@ -1723,13 +1971,546 @@
       <c r="D31" t="s">
         <v>45</v>
       </c>
+      <c r="N31">
+        <f t="shared" si="0"/>
+        <v>-1.1199999062228017E-4</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" t="s">
+        <v>6</v>
+      </c>
+      <c r="J35" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" t="s">
+        <v>8</v>
+      </c>
+      <c r="N35" t="s">
+        <v>64</v>
+      </c>
+      <c r="O35" t="s">
+        <v>65</v>
+      </c>
+      <c r="P35" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36">
+        <v>22.366</v>
+      </c>
+      <c r="D36" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>1.8869500000000001E-2</v>
+      </c>
+      <c r="J36">
+        <v>18.783000000000001</v>
+      </c>
+      <c r="K36" t="s">
+        <v>57</v>
+      </c>
+      <c r="N36">
+        <f>B36-B20</f>
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <f>C36-C20</f>
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <f>I36-I20</f>
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <f>J36-J20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37">
+        <v>13.147</v>
+      </c>
+      <c r="D37" t="s">
+        <v>55</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>2.17725E-2</v>
+      </c>
+      <c r="J37">
+        <v>12.215999999999999</v>
+      </c>
+      <c r="K37" t="s">
+        <v>58</v>
+      </c>
+      <c r="N37">
+        <f t="shared" ref="N37:N47" si="4">B37-B21</f>
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <f t="shared" ref="O37:O47" si="5">C37-C21</f>
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <f t="shared" ref="P37:P47" si="6">I37-I21</f>
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" ref="Q37:Q47" si="7">J37-J21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <v>8.7750000000000004</v>
+      </c>
+      <c r="D38" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <v>2.46755E-2</v>
+      </c>
+      <c r="J38">
+        <v>8.1630000000000003</v>
+      </c>
+      <c r="K38" t="s">
+        <v>59</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39">
+        <v>1376.7230784999999</v>
+      </c>
+      <c r="C39">
+        <v>6.8109999999999999</v>
+      </c>
+      <c r="D39" t="s">
+        <v>38</v>
+      </c>
+      <c r="H39">
+        <v>3</v>
+      </c>
+      <c r="I39">
+        <v>2.903E-2</v>
+      </c>
+      <c r="J39">
+        <v>6.0439999999999996</v>
+      </c>
+      <c r="K39" t="s">
+        <v>39</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>1619.6742099999999</v>
+      </c>
+      <c r="C40">
+        <v>6.0439999999999996</v>
+      </c>
+      <c r="D40" t="s">
+        <v>39</v>
+      </c>
+      <c r="H40">
+        <v>4</v>
+      </c>
+      <c r="I40">
+        <v>2.903E-2</v>
+      </c>
+      <c r="J40">
+        <v>6.0439999999999996</v>
+      </c>
+      <c r="K40" t="s">
+        <v>39</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>1619.6742099999999</v>
+      </c>
+      <c r="C41">
+        <v>6.0439999999999996</v>
+      </c>
+      <c r="D41" t="s">
+        <v>39</v>
+      </c>
+      <c r="H41">
+        <v>5</v>
+      </c>
+      <c r="I41">
+        <v>3.3384499999999998E-2</v>
+      </c>
+      <c r="J41">
+        <v>7.9050000000000002</v>
+      </c>
+      <c r="K41" t="s">
+        <v>60</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42">
+        <v>2105.5764730000001</v>
+      </c>
+      <c r="C42">
+        <v>7.3620000000000001</v>
+      </c>
+      <c r="D42" t="s">
+        <v>40</v>
+      </c>
+      <c r="H42">
+        <v>6</v>
+      </c>
+      <c r="I42">
+        <v>3.62875E-2</v>
+      </c>
+      <c r="J42">
+        <v>11.025</v>
+      </c>
+      <c r="K42" t="s">
+        <v>61</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="B43">
+        <v>2591.478736</v>
+      </c>
+      <c r="C43">
+        <v>9.5269999999999992</v>
+      </c>
+      <c r="D43" t="s">
+        <v>41</v>
+      </c>
+      <c r="H43">
+        <v>7</v>
+      </c>
+      <c r="I43">
+        <v>3.9190500000000003E-2</v>
+      </c>
+      <c r="J43">
+        <v>15.467000000000001</v>
+      </c>
+      <c r="K43" t="s">
+        <v>62</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44">
+        <v>3077.380999</v>
+      </c>
+      <c r="C44">
+        <v>11.606</v>
+      </c>
+      <c r="D44" t="s">
+        <v>42</v>
+      </c>
+      <c r="H44">
+        <v>8</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J44">
+        <v>21.103000000000002</v>
+      </c>
+      <c r="K44" t="s">
+        <v>63</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45">
+        <v>3563.2832619999999</v>
+      </c>
+      <c r="C45">
+        <v>13.420999999999999</v>
+      </c>
+      <c r="D45" t="s">
+        <v>43</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>10</v>
+      </c>
+      <c r="B46">
+        <v>4049.1855249999999</v>
+      </c>
+      <c r="C46">
+        <v>14.973000000000001</v>
+      </c>
+      <c r="D46" t="s">
+        <v>44</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>11</v>
+      </c>
+      <c r="B47">
+        <v>4535.0877879999998</v>
+      </c>
+      <c r="C47">
+        <v>16.295999999999999</v>
+      </c>
+      <c r="D47" t="s">
+        <v>56</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A18:L18"/>
+    <mergeCell ref="A34:L34"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>